<commit_message>
control board működik, clean
</commit_message>
<xml_diff>
--- a/Info/port_konfig.xlsx
+++ b/Info/port_konfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>motor_1_pulse</t>
   </si>
@@ -61,18 +61,6 @@
     <t>USART_1_RX</t>
   </si>
   <si>
-    <t>GOMB_4</t>
-  </si>
-  <si>
-    <t>GOMB_3</t>
-  </si>
-  <si>
-    <t>GOMB_1</t>
-  </si>
-  <si>
-    <t>GOMB_2</t>
-  </si>
-  <si>
     <t>GPIO_IN_INT_6</t>
   </si>
   <si>
@@ -119,6 +107,36 @@
   </si>
   <si>
     <t>5v tolerant no pullup?</t>
+  </si>
+  <si>
+    <t>GOMB_UP</t>
+  </si>
+  <si>
+    <t>GOMB_DOWN</t>
+  </si>
+  <si>
+    <t>GOMB_ENTER</t>
+  </si>
+  <si>
+    <t>GOMB_MODE</t>
+  </si>
+  <si>
+    <t>DOMB_DOWN</t>
+  </si>
+  <si>
+    <t>SR_DATA</t>
+  </si>
+  <si>
+    <t>SR_LATCH</t>
+  </si>
+  <si>
+    <t>SR_CLOCK</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
@@ -148,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,16 +174,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -196,7 +268,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1126587</xdr:colOff>
+      <xdr:colOff>310799</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>71621</xdr:rowOff>
     </xdr:to>
@@ -520,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B15:N26"/>
+  <dimension ref="B15:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -533,8 +605,10 @@
     <col min="3" max="3" width="41" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.21875" style="1" customWidth="1"/>
-    <col min="6" max="9" width="12.6640625" style="1"/>
-    <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="38.5546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="5.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="32.109375" style="1" customWidth="1"/>
@@ -545,10 +619,10 @@
     <row r="15" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -560,17 +634,17 @@
         <v>8</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -582,17 +656,17 @@
         <v>7</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N16" s="2"/>
     </row>
     <row r="18" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>4</v>
@@ -601,10 +675,10 @@
     <row r="19" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>4</v>
@@ -616,17 +690,17 @@
         <v>9</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>4</v>
@@ -635,10 +709,10 @@
     <row r="21" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>4</v>
@@ -650,7 +724,7 @@
         <v>6</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N21" s="2"/>
     </row>
@@ -662,20 +736,20 @@
         <v>5</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>1</v>
@@ -684,20 +758,20 @@
         <v>3</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>2</v>
@@ -706,33 +780,132 @@
         <v>0</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="3"/>
+      <c r="K38" s="1" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="39" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="4"/>
+      <c r="K39" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="4"/>
+      <c r="K40" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J41" s="5"/>
+      <c r="K41" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="K44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="K45" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="K46" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="6:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="K50" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="4"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="5:11" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F55" s="5"/>
+      <c r="I55" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
s curve vezerles v0 mukodik
</commit_message>
<xml_diff>
--- a/Info/port_konfig.xlsx
+++ b/Info/port_konfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>motor_1_pulse</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>ALSO MOTOR</t>
+  </si>
+  <si>
+    <t>dmx rx</t>
   </si>
 </sst>
 </file>
@@ -603,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="D43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -912,6 +915,9 @@
       </c>
       <c r="F52" s="4"/>
       <c r="I52" s="4"/>
+      <c r="K52" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="53" spans="5:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F53" s="4"/>

</xml_diff>

<commit_message>
reset funkcio kesz + tilt motor kesz
</commit_message>
<xml_diff>
--- a/Info/port_konfig.xlsx
+++ b/Info/port_konfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>motor_1_pulse</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">pan 0 </t>
+  </si>
+  <si>
+    <t>MOTOR_2_DIRECTION</t>
+  </si>
+  <si>
+    <t>MOTOR_2_PULSE</t>
   </si>
 </sst>
 </file>
@@ -618,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -884,6 +890,9 @@
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="I44" s="4"/>
       <c r="K44" s="1" t="s">
@@ -891,6 +900,9 @@
       </c>
     </row>
     <row r="45" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="I45" s="4"/>
       <c r="K45" s="1" t="s">

</xml_diff>

<commit_message>
relé engedélyezés hozzá adva
</commit_message>
<xml_diff>
--- a/Info/port_konfig.xlsx
+++ b/Info/port_konfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>motor_1_pulse</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>MOTOR_2_PULSE</t>
+  </si>
+  <si>
+    <t>RELÉ</t>
   </si>
 </sst>
 </file>
@@ -624,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="E39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -881,6 +884,9 @@
       </c>
       <c r="F42" s="3"/>
       <c r="I42" s="3"/>
+      <c r="K42" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="43" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E43" s="1" t="s">

</xml_diff>